<commit_message>
Clean up & add metadata
</commit_message>
<xml_diff>
--- a/RedoxParsePlot/ExampleData/HypnosLogger076_DataChannelsInfo.xlsx
+++ b/RedoxParsePlot/ExampleData/HypnosLogger076_DataChannelsInfo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6820" yWindow="0" windowWidth="21900" windowHeight="11220" tabRatio="500"/>
+    <workbookView xWindow="-1300" yWindow="-24000" windowWidth="20080" windowHeight="17720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>ChannelID</t>
   </si>
@@ -180,23 +180,25 @@
     <t>New Hypnos Logger (#076) installed Oct 5, 2012 at 13:00 EST.  All logger times in Eastern Standard Time (EST, UTC-5)</t>
   </si>
   <si>
-    <t>DistanceFromSensorTip_cm</t>
-  </si>
-  <si>
-    <t>SensorCode</t>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Sensor EquipmentCode</t>
+  </si>
+  <si>
+    <t>DistanceFromProbeTip_cm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <u/>
@@ -213,6 +215,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -232,7 +239,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -248,14 +255,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -263,6 +285,13 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -270,6 +299,13 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -599,21 +635,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35:F43"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -621,7 +660,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -629,12 +668,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -642,7 +681,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -650,7 +689,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="26">
+    <row r="7" spans="1:8" s="1" customFormat="1" ht="39">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,13 +706,16 @@
         <v>54</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>0</v>
       </c>
@@ -684,10 +726,14 @@
         <v>44</v>
       </c>
       <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2">
+        <f>130-28-F8</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>1</v>
       </c>
@@ -698,10 +744,14 @@
         <v>44</v>
       </c>
       <c r="F9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>7</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" ref="G9:G43" si="0">130-28-F9</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>2</v>
       </c>
@@ -712,10 +762,14 @@
         <v>44</v>
       </c>
       <c r="F10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>12</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>3</v>
       </c>
@@ -726,10 +780,14 @@
         <v>44</v>
       </c>
       <c r="F11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>17</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>4</v>
       </c>
@@ -740,10 +798,14 @@
         <v>44</v>
       </c>
       <c r="F12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>22</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>5</v>
       </c>
@@ -754,10 +816,14 @@
         <v>44</v>
       </c>
       <c r="F13">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>27</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>6</v>
       </c>
@@ -768,10 +834,14 @@
         <v>44</v>
       </c>
       <c r="F14">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>32</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>7</v>
       </c>
@@ -782,10 +852,14 @@
         <v>44</v>
       </c>
       <c r="F15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>42</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>8</v>
       </c>
@@ -796,10 +870,14 @@
         <v>44</v>
       </c>
       <c r="F16">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>9</v>
       </c>
@@ -810,10 +888,14 @@
         <v>45</v>
       </c>
       <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="G17" s="2">
+        <f>130-28-F17</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>10</v>
       </c>
@@ -824,10 +906,14 @@
         <v>45</v>
       </c>
       <c r="F18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>7</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>11</v>
       </c>
@@ -838,10 +924,14 @@
         <v>45</v>
       </c>
       <c r="F19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>12</v>
       </c>
@@ -852,10 +942,14 @@
         <v>45</v>
       </c>
       <c r="F20">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>13</v>
       </c>
@@ -866,10 +960,14 @@
         <v>45</v>
       </c>
       <c r="F21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>22</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>14</v>
       </c>
@@ -880,10 +978,14 @@
         <v>45</v>
       </c>
       <c r="F22">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>27</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>15</v>
       </c>
@@ -894,10 +996,14 @@
         <v>45</v>
       </c>
       <c r="F23">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>32</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>16</v>
       </c>
@@ -908,10 +1014,14 @@
         <v>45</v>
       </c>
       <c r="F24">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>42</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>17</v>
       </c>
@@ -922,10 +1032,14 @@
         <v>45</v>
       </c>
       <c r="F25">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>18</v>
       </c>
@@ -936,10 +1050,14 @@
         <v>46</v>
       </c>
       <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="G26" s="2">
+        <f>130-28-F26</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>19</v>
       </c>
@@ -950,10 +1068,14 @@
         <v>46</v>
       </c>
       <c r="F27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>7</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>20</v>
       </c>
@@ -964,10 +1086,14 @@
         <v>46</v>
       </c>
       <c r="F28">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>21</v>
       </c>
@@ -978,10 +1104,14 @@
         <v>46</v>
       </c>
       <c r="F29">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>22</v>
       </c>
@@ -992,10 +1122,14 @@
         <v>46</v>
       </c>
       <c r="F30">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>22</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>23</v>
       </c>
@@ -1006,10 +1140,14 @@
         <v>46</v>
       </c>
       <c r="F31">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>27</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>24</v>
       </c>
@@ -1020,10 +1158,14 @@
         <v>46</v>
       </c>
       <c r="F32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>32</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33">
         <v>25</v>
       </c>
@@ -1034,10 +1176,14 @@
         <v>46</v>
       </c>
       <c r="F33">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>42</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34">
         <v>26</v>
       </c>
@@ -1048,10 +1194,14 @@
         <v>46</v>
       </c>
       <c r="F34">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35">
         <v>27</v>
       </c>
@@ -1062,10 +1212,14 @@
         <v>47</v>
       </c>
       <c r="F35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="G35" s="2">
+        <f>130-28-F35</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36">
         <v>28</v>
       </c>
@@ -1076,10 +1230,14 @@
         <v>47</v>
       </c>
       <c r="F36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>7</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="0"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37">
         <v>29</v>
       </c>
@@ -1090,10 +1248,14 @@
         <v>47</v>
       </c>
       <c r="F37">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38">
         <v>30</v>
       </c>
@@ -1104,10 +1266,14 @@
         <v>47</v>
       </c>
       <c r="F38">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>17</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="0"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39">
         <v>31</v>
       </c>
@@ -1118,10 +1284,14 @@
         <v>47</v>
       </c>
       <c r="F39">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>22</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40">
         <v>32</v>
       </c>
@@ -1132,10 +1302,14 @@
         <v>47</v>
       </c>
       <c r="F40">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>27</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41">
         <v>33</v>
       </c>
@@ -1146,10 +1320,14 @@
         <v>47</v>
       </c>
       <c r="F41">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>32</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42">
         <v>34</v>
       </c>
@@ -1160,10 +1338,14 @@
         <v>47</v>
       </c>
       <c r="F42">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>42</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43">
         <v>35</v>
       </c>
@@ -1174,7 +1356,11 @@
         <v>47</v>
       </c>
       <c r="F43">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>